<commit_message>
First edition of the bot working
</commit_message>
<xml_diff>
--- a/files/info.xlsx
+++ b/files/info.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-640" yWindow="-18420" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
+    <workbookView minimized="1" xWindow="0" yWindow="4060" windowWidth="25600" windowHeight="12840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,18 +27,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>team1</t>
-  </si>
-  <si>
-    <t>t1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>team2</t>
   </si>
   <si>
-    <t>t2</t>
+    <t>Information de la première team</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>VP</t>
+  </si>
+  <si>
+    <t>Astralis</t>
   </si>
 </sst>
 </file>
@@ -353,33 +359,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="55.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1">
         <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
         <v>3</v>
       </c>
     </row>

</xml_diff>